<commit_message>
Added new classes in input file and re-generated the view.
</commit_message>
<xml_diff>
--- a/src/main/resources/OBI-ISAview/OBI-ISAview.xlsx
+++ b/src/main/resources/OBI-ISAview/OBI-ISAview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40600" windowHeight="25980"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7511" uniqueCount="7507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7537" uniqueCount="7520">
   <si>
     <t>Source ontology term IRI</t>
   </si>
@@ -22541,13 +22541,52 @@
   </si>
   <si>
     <t>sample, extract, labeled extract</t>
+  </si>
+  <si>
+    <t>unplanned occurrence effecting an study</t>
+  </si>
+  <si>
+    <t>study agent role</t>
+  </si>
+  <si>
+    <t>study results report</t>
+  </si>
+  <si>
+    <t>hypothesis driven study</t>
+  </si>
+  <si>
+    <t>hypothesis generating study</t>
+  </si>
+  <si>
+    <t>study description</t>
+  </si>
+  <si>
+    <t>study title</t>
+  </si>
+  <si>
+    <t>study identifier</t>
+  </si>
+  <si>
+    <t>publication about a study</t>
+  </si>
+  <si>
+    <t>introduction to a publication about a study</t>
+  </si>
+  <si>
+    <t>discussion section of a publication about a study</t>
+  </si>
+  <si>
+    <t>study design type</t>
+  </si>
+  <si>
+    <t>study protocol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -22557,6 +22596,18 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -22577,8 +22628,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -22587,7 +22642,11 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -22884,8 +22943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3749"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1592" workbookViewId="0">
-      <selection activeCell="D1620" sqref="D1620"/>
+    <sheetView tabSelected="1" topLeftCell="A1695" workbookViewId="0">
+      <selection activeCell="D1734" sqref="D1734"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -25726,7 +25785,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="353" spans="1:2">
+    <row r="353" spans="1:4">
       <c r="A353" t="s">
         <v>707</v>
       </c>
@@ -25734,7 +25793,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="354" spans="1:2">
+    <row r="354" spans="1:4">
       <c r="A354" t="s">
         <v>709</v>
       </c>
@@ -25742,7 +25801,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="355" spans="1:2">
+    <row r="355" spans="1:4">
       <c r="A355" t="s">
         <v>711</v>
       </c>
@@ -25750,7 +25809,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="356" spans="1:2">
+    <row r="356" spans="1:4">
       <c r="A356" t="s">
         <v>713</v>
       </c>
@@ -25758,15 +25817,21 @@
         <v>714</v>
       </c>
     </row>
-    <row r="357" spans="1:2">
+    <row r="357" spans="1:4">
       <c r="A357" t="s">
         <v>715</v>
       </c>
       <c r="B357" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="358" spans="1:2">
+      <c r="C357" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D357" t="s">
+        <v>7515</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4">
       <c r="A358" t="s">
         <v>717</v>
       </c>
@@ -25774,7 +25839,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="359" spans="1:2">
+    <row r="359" spans="1:4">
       <c r="A359" t="s">
         <v>719</v>
       </c>
@@ -25782,7 +25847,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="360" spans="1:2">
+    <row r="360" spans="1:4">
       <c r="A360" t="s">
         <v>721</v>
       </c>
@@ -25790,15 +25855,21 @@
         <v>722</v>
       </c>
     </row>
-    <row r="361" spans="1:2">
+    <row r="361" spans="1:4">
       <c r="A361" t="s">
         <v>723</v>
       </c>
       <c r="B361" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="362" spans="1:2">
+      <c r="C361" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D361" t="s">
+        <v>7516</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4">
       <c r="A362" t="s">
         <v>725</v>
       </c>
@@ -25806,7 +25877,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="363" spans="1:2">
+    <row r="363" spans="1:4">
       <c r="A363" t="s">
         <v>727</v>
       </c>
@@ -25814,15 +25885,21 @@
         <v>728</v>
       </c>
     </row>
-    <row r="364" spans="1:2">
+    <row r="364" spans="1:4">
       <c r="A364" t="s">
         <v>729</v>
       </c>
       <c r="B364" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="365" spans="1:2">
+      <c r="C364" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D364" t="s">
+        <v>7517</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4">
       <c r="A365" t="s">
         <v>731</v>
       </c>
@@ -25830,7 +25907,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="366" spans="1:2">
+    <row r="366" spans="1:4">
       <c r="A366" t="s">
         <v>733</v>
       </c>
@@ -25838,7 +25915,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="367" spans="1:2">
+    <row r="367" spans="1:4">
       <c r="A367" t="s">
         <v>735</v>
       </c>
@@ -25846,7 +25923,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="368" spans="1:2">
+    <row r="368" spans="1:4">
       <c r="A368" t="s">
         <v>737</v>
       </c>
@@ -35978,7 +36055,7 @@
         <v>7502</v>
       </c>
     </row>
-    <row r="1633" spans="1:2">
+    <row r="1633" spans="1:4">
       <c r="A1633" t="s">
         <v>3267</v>
       </c>
@@ -35986,7 +36063,7 @@
         <v>3268</v>
       </c>
     </row>
-    <row r="1634" spans="1:2">
+    <row r="1634" spans="1:4">
       <c r="A1634" t="s">
         <v>3269</v>
       </c>
@@ -35994,7 +36071,7 @@
         <v>3270</v>
       </c>
     </row>
-    <row r="1635" spans="1:2">
+    <row r="1635" spans="1:4">
       <c r="A1635" t="s">
         <v>3271</v>
       </c>
@@ -36002,7 +36079,7 @@
         <v>3272</v>
       </c>
     </row>
-    <row r="1636" spans="1:2">
+    <row r="1636" spans="1:4">
       <c r="A1636" t="s">
         <v>3273</v>
       </c>
@@ -36010,7 +36087,7 @@
         <v>3274</v>
       </c>
     </row>
-    <row r="1637" spans="1:2">
+    <row r="1637" spans="1:4">
       <c r="A1637" t="s">
         <v>3275</v>
       </c>
@@ -36018,7 +36095,7 @@
         <v>3276</v>
       </c>
     </row>
-    <row r="1638" spans="1:2">
+    <row r="1638" spans="1:4">
       <c r="A1638" t="s">
         <v>3277</v>
       </c>
@@ -36026,15 +36103,21 @@
         <v>3278</v>
       </c>
     </row>
-    <row r="1639" spans="1:2">
+    <row r="1639" spans="1:4">
       <c r="A1639" t="s">
         <v>3279</v>
       </c>
       <c r="B1639" t="s">
         <v>3280</v>
       </c>
-    </row>
-    <row r="1640" spans="1:2">
+      <c r="C1639" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D1639" t="s">
+        <v>7507</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:4">
       <c r="A1640" t="s">
         <v>3281</v>
       </c>
@@ -36042,7 +36125,7 @@
         <v>3282</v>
       </c>
     </row>
-    <row r="1641" spans="1:2">
+    <row r="1641" spans="1:4">
       <c r="A1641" t="s">
         <v>3283</v>
       </c>
@@ -36050,7 +36133,7 @@
         <v>3284</v>
       </c>
     </row>
-    <row r="1642" spans="1:2">
+    <row r="1642" spans="1:4">
       <c r="A1642" t="s">
         <v>3285</v>
       </c>
@@ -36058,7 +36141,7 @@
         <v>3286</v>
       </c>
     </row>
-    <row r="1643" spans="1:2">
+    <row r="1643" spans="1:4">
       <c r="A1643" t="s">
         <v>3287</v>
       </c>
@@ -36066,7 +36149,7 @@
         <v>3288</v>
       </c>
     </row>
-    <row r="1644" spans="1:2">
+    <row r="1644" spans="1:4">
       <c r="A1644" t="s">
         <v>3289</v>
       </c>
@@ -36074,7 +36157,7 @@
         <v>3290</v>
       </c>
     </row>
-    <row r="1645" spans="1:2">
+    <row r="1645" spans="1:4">
       <c r="A1645" t="s">
         <v>3291</v>
       </c>
@@ -36082,7 +36165,7 @@
         <v>3292</v>
       </c>
     </row>
-    <row r="1646" spans="1:2">
+    <row r="1646" spans="1:4">
       <c r="A1646" t="s">
         <v>3293</v>
       </c>
@@ -36090,7 +36173,7 @@
         <v>3294</v>
       </c>
     </row>
-    <row r="1647" spans="1:2">
+    <row r="1647" spans="1:4">
       <c r="A1647" t="s">
         <v>3295</v>
       </c>
@@ -36098,7 +36181,7 @@
         <v>3296</v>
       </c>
     </row>
-    <row r="1648" spans="1:2">
+    <row r="1648" spans="1:4">
       <c r="A1648" t="s">
         <v>3297</v>
       </c>
@@ -36490,7 +36573,7 @@
         <v>3394</v>
       </c>
     </row>
-    <row r="1697" spans="1:2">
+    <row r="1697" spans="1:4">
       <c r="A1697" t="s">
         <v>3395</v>
       </c>
@@ -36498,7 +36581,7 @@
         <v>3396</v>
       </c>
     </row>
-    <row r="1698" spans="1:2">
+    <row r="1698" spans="1:4">
       <c r="A1698" t="s">
         <v>3397</v>
       </c>
@@ -36506,7 +36589,7 @@
         <v>3398</v>
       </c>
     </row>
-    <row r="1699" spans="1:2">
+    <row r="1699" spans="1:4">
       <c r="A1699" t="s">
         <v>3399</v>
       </c>
@@ -36514,15 +36597,21 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="1700" spans="1:2">
+    <row r="1700" spans="1:4">
       <c r="A1700" t="s">
         <v>3401</v>
       </c>
       <c r="B1700" t="s">
         <v>3402</v>
       </c>
-    </row>
-    <row r="1701" spans="1:2">
+      <c r="C1700" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D1700" t="s">
+        <v>7508</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:4">
       <c r="A1701" t="s">
         <v>3403</v>
       </c>
@@ -36530,7 +36619,7 @@
         <v>3404</v>
       </c>
     </row>
-    <row r="1702" spans="1:2">
+    <row r="1702" spans="1:4">
       <c r="A1702" t="s">
         <v>3405</v>
       </c>
@@ -36538,7 +36627,7 @@
         <v>3406</v>
       </c>
     </row>
-    <row r="1703" spans="1:2">
+    <row r="1703" spans="1:4">
       <c r="A1703" t="s">
         <v>3407</v>
       </c>
@@ -36546,7 +36635,7 @@
         <v>3408</v>
       </c>
     </row>
-    <row r="1704" spans="1:2">
+    <row r="1704" spans="1:4">
       <c r="A1704" t="s">
         <v>3409</v>
       </c>
@@ -36554,7 +36643,7 @@
         <v>3410</v>
       </c>
     </row>
-    <row r="1705" spans="1:2">
+    <row r="1705" spans="1:4">
       <c r="A1705" t="s">
         <v>3411</v>
       </c>
@@ -36562,7 +36651,7 @@
         <v>3412</v>
       </c>
     </row>
-    <row r="1706" spans="1:2">
+    <row r="1706" spans="1:4">
       <c r="A1706" t="s">
         <v>3413</v>
       </c>
@@ -36570,7 +36659,7 @@
         <v>3414</v>
       </c>
     </row>
-    <row r="1707" spans="1:2">
+    <row r="1707" spans="1:4">
       <c r="A1707" t="s">
         <v>3415</v>
       </c>
@@ -36578,7 +36667,7 @@
         <v>3416</v>
       </c>
     </row>
-    <row r="1708" spans="1:2">
+    <row r="1708" spans="1:4">
       <c r="A1708" t="s">
         <v>3417</v>
       </c>
@@ -36586,15 +36675,21 @@
         <v>3418</v>
       </c>
     </row>
-    <row r="1709" spans="1:2">
+    <row r="1709" spans="1:4">
       <c r="A1709" t="s">
         <v>3419</v>
       </c>
       <c r="B1709" t="s">
         <v>3420</v>
       </c>
-    </row>
-    <row r="1710" spans="1:2">
+      <c r="C1709" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D1709" t="s">
+        <v>7509</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:4">
       <c r="A1710" t="s">
         <v>3421</v>
       </c>
@@ -36602,7 +36697,7 @@
         <v>3422</v>
       </c>
     </row>
-    <row r="1711" spans="1:2">
+    <row r="1711" spans="1:4">
       <c r="A1711" t="s">
         <v>3423</v>
       </c>
@@ -36610,7 +36705,7 @@
         <v>3424</v>
       </c>
     </row>
-    <row r="1712" spans="1:2">
+    <row r="1712" spans="1:4">
       <c r="A1712" t="s">
         <v>3425</v>
       </c>
@@ -36746,7 +36841,7 @@
         <v>3458</v>
       </c>
     </row>
-    <row r="1729" spans="1:2">
+    <row r="1729" spans="1:4">
       <c r="A1729" t="s">
         <v>3459</v>
       </c>
@@ -36754,7 +36849,7 @@
         <v>3460</v>
       </c>
     </row>
-    <row r="1730" spans="1:2">
+    <row r="1730" spans="1:4">
       <c r="A1730" t="s">
         <v>3461</v>
       </c>
@@ -36762,7 +36857,7 @@
         <v>3462</v>
       </c>
     </row>
-    <row r="1731" spans="1:2">
+    <row r="1731" spans="1:4">
       <c r="A1731" t="s">
         <v>3463</v>
       </c>
@@ -36770,7 +36865,7 @@
         <v>3464</v>
       </c>
     </row>
-    <row r="1732" spans="1:2">
+    <row r="1732" spans="1:4">
       <c r="A1732" t="s">
         <v>3465</v>
       </c>
@@ -36778,15 +36873,21 @@
         <v>3466</v>
       </c>
     </row>
-    <row r="1733" spans="1:2">
+    <row r="1733" spans="1:4">
       <c r="A1733" t="s">
         <v>3467</v>
       </c>
       <c r="B1733" t="s">
         <v>3468</v>
       </c>
-    </row>
-    <row r="1734" spans="1:2">
+      <c r="C1733" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D1733" t="s">
+        <v>7519</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:4">
       <c r="A1734" t="s">
         <v>3469</v>
       </c>
@@ -36794,7 +36895,7 @@
         <v>3470</v>
       </c>
     </row>
-    <row r="1735" spans="1:2">
+    <row r="1735" spans="1:4">
       <c r="A1735" t="s">
         <v>3471</v>
       </c>
@@ -36802,7 +36903,7 @@
         <v>3472</v>
       </c>
     </row>
-    <row r="1736" spans="1:2">
+    <row r="1736" spans="1:4">
       <c r="A1736" t="s">
         <v>3473</v>
       </c>
@@ -36810,7 +36911,7 @@
         <v>3474</v>
       </c>
     </row>
-    <row r="1737" spans="1:2">
+    <row r="1737" spans="1:4">
       <c r="A1737" t="s">
         <v>3475</v>
       </c>
@@ -36818,7 +36919,7 @@
         <v>3476</v>
       </c>
     </row>
-    <row r="1738" spans="1:2">
+    <row r="1738" spans="1:4">
       <c r="A1738" t="s">
         <v>3477</v>
       </c>
@@ -36826,7 +36927,7 @@
         <v>3478</v>
       </c>
     </row>
-    <row r="1739" spans="1:2">
+    <row r="1739" spans="1:4">
       <c r="A1739" t="s">
         <v>3479</v>
       </c>
@@ -36834,7 +36935,7 @@
         <v>3480</v>
       </c>
     </row>
-    <row r="1740" spans="1:2">
+    <row r="1740" spans="1:4">
       <c r="A1740" t="s">
         <v>3481</v>
       </c>
@@ -36842,7 +36943,7 @@
         <v>3482</v>
       </c>
     </row>
-    <row r="1741" spans="1:2">
+    <row r="1741" spans="1:4">
       <c r="A1741" t="s">
         <v>3483</v>
       </c>
@@ -36850,7 +36951,7 @@
         <v>3484</v>
       </c>
     </row>
-    <row r="1742" spans="1:2">
+    <row r="1742" spans="1:4">
       <c r="A1742" t="s">
         <v>3485</v>
       </c>
@@ -36858,7 +36959,7 @@
         <v>3486</v>
       </c>
     </row>
-    <row r="1743" spans="1:2">
+    <row r="1743" spans="1:4">
       <c r="A1743" t="s">
         <v>3487</v>
       </c>
@@ -36866,7 +36967,7 @@
         <v>3488</v>
       </c>
     </row>
-    <row r="1744" spans="1:2">
+    <row r="1744" spans="1:4">
       <c r="A1744" t="s">
         <v>3489</v>
       </c>
@@ -36874,7 +36975,7 @@
         <v>3490</v>
       </c>
     </row>
-    <row r="1745" spans="1:2">
+    <row r="1745" spans="1:4">
       <c r="A1745" t="s">
         <v>3491</v>
       </c>
@@ -36882,7 +36983,7 @@
         <v>3492</v>
       </c>
     </row>
-    <row r="1746" spans="1:2">
+    <row r="1746" spans="1:4">
       <c r="A1746" t="s">
         <v>3493</v>
       </c>
@@ -36890,7 +36991,7 @@
         <v>3494</v>
       </c>
     </row>
-    <row r="1747" spans="1:2">
+    <row r="1747" spans="1:4">
       <c r="A1747" t="s">
         <v>3495</v>
       </c>
@@ -36898,7 +36999,7 @@
         <v>3496</v>
       </c>
     </row>
-    <row r="1748" spans="1:2">
+    <row r="1748" spans="1:4">
       <c r="A1748" t="s">
         <v>3497</v>
       </c>
@@ -36906,7 +37007,7 @@
         <v>3498</v>
       </c>
     </row>
-    <row r="1749" spans="1:2">
+    <row r="1749" spans="1:4">
       <c r="A1749" t="s">
         <v>3499</v>
       </c>
@@ -36914,7 +37015,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="1750" spans="1:2">
+    <row r="1750" spans="1:4">
       <c r="A1750" t="s">
         <v>3501</v>
       </c>
@@ -36922,7 +37023,7 @@
         <v>3502</v>
       </c>
     </row>
-    <row r="1751" spans="1:2">
+    <row r="1751" spans="1:4">
       <c r="A1751" t="s">
         <v>3503</v>
       </c>
@@ -36930,7 +37031,7 @@
         <v>3504</v>
       </c>
     </row>
-    <row r="1752" spans="1:2">
+    <row r="1752" spans="1:4">
       <c r="A1752" t="s">
         <v>3505</v>
       </c>
@@ -36938,7 +37039,7 @@
         <v>3506</v>
       </c>
     </row>
-    <row r="1753" spans="1:2">
+    <row r="1753" spans="1:4">
       <c r="A1753" t="s">
         <v>3507</v>
       </c>
@@ -36946,7 +37047,7 @@
         <v>3508</v>
       </c>
     </row>
-    <row r="1754" spans="1:2">
+    <row r="1754" spans="1:4">
       <c r="A1754" t="s">
         <v>3509</v>
       </c>
@@ -36954,7 +37055,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="1755" spans="1:2">
+    <row r="1755" spans="1:4">
       <c r="A1755" t="s">
         <v>3511</v>
       </c>
@@ -36962,7 +37063,7 @@
         <v>3512</v>
       </c>
     </row>
-    <row r="1756" spans="1:2">
+    <row r="1756" spans="1:4">
       <c r="A1756" t="s">
         <v>3513</v>
       </c>
@@ -36970,23 +37071,35 @@
         <v>3514</v>
       </c>
     </row>
-    <row r="1757" spans="1:2">
+    <row r="1757" spans="1:4">
       <c r="A1757" t="s">
         <v>3515</v>
       </c>
       <c r="B1757" t="s">
         <v>3516</v>
       </c>
-    </row>
-    <row r="1758" spans="1:2">
+      <c r="C1757" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D1757" t="s">
+        <v>7510</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:4">
       <c r="A1758" t="s">
         <v>3517</v>
       </c>
       <c r="B1758" t="s">
         <v>3518</v>
       </c>
-    </row>
-    <row r="1759" spans="1:2">
+      <c r="C1758" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D1758" t="s">
+        <v>7511</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:4">
       <c r="A1759" t="s">
         <v>3519</v>
       </c>
@@ -36994,7 +37107,7 @@
         <v>3520</v>
       </c>
     </row>
-    <row r="1760" spans="1:2">
+    <row r="1760" spans="1:4">
       <c r="A1760" t="s">
         <v>3521</v>
       </c>
@@ -45974,7 +46087,7 @@
         <v>5762</v>
       </c>
     </row>
-    <row r="2881" spans="1:2">
+    <row r="2881" spans="1:4">
       <c r="A2881" t="s">
         <v>5763</v>
       </c>
@@ -45982,7 +46095,7 @@
         <v>5764</v>
       </c>
     </row>
-    <row r="2882" spans="1:2">
+    <row r="2882" spans="1:4">
       <c r="A2882" t="s">
         <v>5765</v>
       </c>
@@ -45990,7 +46103,7 @@
         <v>5766</v>
       </c>
     </row>
-    <row r="2883" spans="1:2">
+    <row r="2883" spans="1:4">
       <c r="A2883" t="s">
         <v>5767</v>
       </c>
@@ -45998,7 +46111,7 @@
         <v>5768</v>
       </c>
     </row>
-    <row r="2884" spans="1:2">
+    <row r="2884" spans="1:4">
       <c r="A2884" t="s">
         <v>5769</v>
       </c>
@@ -46006,7 +46119,7 @@
         <v>5770</v>
       </c>
     </row>
-    <row r="2885" spans="1:2">
+    <row r="2885" spans="1:4">
       <c r="A2885" t="s">
         <v>5771</v>
       </c>
@@ -46014,7 +46127,7 @@
         <v>5772</v>
       </c>
     </row>
-    <row r="2886" spans="1:2">
+    <row r="2886" spans="1:4">
       <c r="A2886" t="s">
         <v>5773</v>
       </c>
@@ -46022,7 +46135,7 @@
         <v>5774</v>
       </c>
     </row>
-    <row r="2887" spans="1:2">
+    <row r="2887" spans="1:4">
       <c r="A2887" t="s">
         <v>5775</v>
       </c>
@@ -46030,7 +46143,7 @@
         <v>5776</v>
       </c>
     </row>
-    <row r="2888" spans="1:2">
+    <row r="2888" spans="1:4">
       <c r="A2888" t="s">
         <v>5777</v>
       </c>
@@ -46038,15 +46151,21 @@
         <v>5778</v>
       </c>
     </row>
-    <row r="2889" spans="1:2">
+    <row r="2889" spans="1:4">
       <c r="A2889" t="s">
         <v>5779</v>
       </c>
       <c r="B2889" t="s">
         <v>5780</v>
       </c>
-    </row>
-    <row r="2890" spans="1:2">
+      <c r="C2889" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D2889" t="s">
+        <v>7512</v>
+      </c>
+    </row>
+    <row r="2890" spans="1:4">
       <c r="A2890" t="s">
         <v>5781</v>
       </c>
@@ -46054,7 +46173,7 @@
         <v>5782</v>
       </c>
     </row>
-    <row r="2891" spans="1:2">
+    <row r="2891" spans="1:4">
       <c r="A2891" t="s">
         <v>5783</v>
       </c>
@@ -46062,7 +46181,7 @@
         <v>5784</v>
       </c>
     </row>
-    <row r="2892" spans="1:2">
+    <row r="2892" spans="1:4">
       <c r="A2892" t="s">
         <v>5785</v>
       </c>
@@ -46070,7 +46189,7 @@
         <v>5786</v>
       </c>
     </row>
-    <row r="2893" spans="1:2">
+    <row r="2893" spans="1:4">
       <c r="A2893" t="s">
         <v>5787</v>
       </c>
@@ -46078,7 +46197,7 @@
         <v>5788</v>
       </c>
     </row>
-    <row r="2894" spans="1:2">
+    <row r="2894" spans="1:4">
       <c r="A2894" t="s">
         <v>5789</v>
       </c>
@@ -46086,7 +46205,7 @@
         <v>5790</v>
       </c>
     </row>
-    <row r="2895" spans="1:2">
+    <row r="2895" spans="1:4">
       <c r="A2895" t="s">
         <v>5791</v>
       </c>
@@ -46094,15 +46213,21 @@
         <v>5792</v>
       </c>
     </row>
-    <row r="2896" spans="1:2">
+    <row r="2896" spans="1:4">
       <c r="A2896" t="s">
         <v>5793</v>
       </c>
       <c r="B2896" t="s">
         <v>5794</v>
       </c>
-    </row>
-    <row r="2897" spans="1:2">
+      <c r="C2896" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D2896" t="s">
+        <v>7513</v>
+      </c>
+    </row>
+    <row r="2897" spans="1:4">
       <c r="A2897" t="s">
         <v>5795</v>
       </c>
@@ -46110,7 +46235,7 @@
         <v>5796</v>
       </c>
     </row>
-    <row r="2898" spans="1:2">
+    <row r="2898" spans="1:4">
       <c r="A2898" t="s">
         <v>5797</v>
       </c>
@@ -46118,7 +46243,7 @@
         <v>5798</v>
       </c>
     </row>
-    <row r="2899" spans="1:2">
+    <row r="2899" spans="1:4">
       <c r="A2899" t="s">
         <v>5799</v>
       </c>
@@ -46126,7 +46251,7 @@
         <v>5800</v>
       </c>
     </row>
-    <row r="2900" spans="1:2">
+    <row r="2900" spans="1:4">
       <c r="A2900" t="s">
         <v>5801</v>
       </c>
@@ -46134,7 +46259,7 @@
         <v>5802</v>
       </c>
     </row>
-    <row r="2901" spans="1:2">
+    <row r="2901" spans="1:4">
       <c r="A2901" t="s">
         <v>5803</v>
       </c>
@@ -46142,15 +46267,21 @@
         <v>5804</v>
       </c>
     </row>
-    <row r="2902" spans="1:2">
+    <row r="2902" spans="1:4">
       <c r="A2902" t="s">
         <v>5805</v>
       </c>
       <c r="B2902" t="s">
         <v>5806</v>
       </c>
-    </row>
-    <row r="2903" spans="1:2">
+      <c r="C2902" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D2902" t="s">
+        <v>7514</v>
+      </c>
+    </row>
+    <row r="2903" spans="1:4">
       <c r="A2903" t="s">
         <v>5807</v>
       </c>
@@ -46158,7 +46289,7 @@
         <v>5808</v>
       </c>
     </row>
-    <row r="2904" spans="1:2">
+    <row r="2904" spans="1:4">
       <c r="A2904" t="s">
         <v>5809</v>
       </c>
@@ -46166,7 +46297,7 @@
         <v>5810</v>
       </c>
     </row>
-    <row r="2905" spans="1:2">
+    <row r="2905" spans="1:4">
       <c r="A2905" t="s">
         <v>5811</v>
       </c>
@@ -46174,7 +46305,7 @@
         <v>5812</v>
       </c>
     </row>
-    <row r="2906" spans="1:2">
+    <row r="2906" spans="1:4">
       <c r="A2906" t="s">
         <v>5813</v>
       </c>
@@ -46182,7 +46313,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="2907" spans="1:2">
+    <row r="2907" spans="1:4">
       <c r="A2907" t="s">
         <v>5815</v>
       </c>
@@ -46190,7 +46321,7 @@
         <v>5816</v>
       </c>
     </row>
-    <row r="2908" spans="1:2">
+    <row r="2908" spans="1:4">
       <c r="A2908" t="s">
         <v>5817</v>
       </c>
@@ -46198,7 +46329,7 @@
         <v>5818</v>
       </c>
     </row>
-    <row r="2909" spans="1:2">
+    <row r="2909" spans="1:4">
       <c r="A2909" t="s">
         <v>5819</v>
       </c>
@@ -46206,7 +46337,7 @@
         <v>5820</v>
       </c>
     </row>
-    <row r="2910" spans="1:2">
+    <row r="2910" spans="1:4">
       <c r="A2910" t="s">
         <v>5821</v>
       </c>
@@ -46214,7 +46345,7 @@
         <v>5822</v>
       </c>
     </row>
-    <row r="2911" spans="1:2">
+    <row r="2911" spans="1:4">
       <c r="A2911" t="s">
         <v>5823</v>
       </c>
@@ -46222,7 +46353,7 @@
         <v>5824</v>
       </c>
     </row>
-    <row r="2912" spans="1:2">
+    <row r="2912" spans="1:4">
       <c r="A2912" t="s">
         <v>5825</v>
       </c>
@@ -49942,7 +50073,7 @@
         <v>6754</v>
       </c>
     </row>
-    <row r="3377" spans="1:2">
+    <row r="3377" spans="1:4">
       <c r="A3377" t="s">
         <v>6755</v>
       </c>
@@ -49950,7 +50081,7 @@
         <v>6756</v>
       </c>
     </row>
-    <row r="3378" spans="1:2">
+    <row r="3378" spans="1:4">
       <c r="A3378" t="s">
         <v>6757</v>
       </c>
@@ -49958,7 +50089,7 @@
         <v>6758</v>
       </c>
     </row>
-    <row r="3379" spans="1:2">
+    <row r="3379" spans="1:4">
       <c r="A3379" t="s">
         <v>6759</v>
       </c>
@@ -49966,7 +50097,7 @@
         <v>6760</v>
       </c>
     </row>
-    <row r="3380" spans="1:2">
+    <row r="3380" spans="1:4">
       <c r="A3380" t="s">
         <v>6761</v>
       </c>
@@ -49974,7 +50105,7 @@
         <v>6762</v>
       </c>
     </row>
-    <row r="3381" spans="1:2">
+    <row r="3381" spans="1:4">
       <c r="A3381" t="s">
         <v>6763</v>
       </c>
@@ -49982,7 +50113,7 @@
         <v>6764</v>
       </c>
     </row>
-    <row r="3382" spans="1:2">
+    <row r="3382" spans="1:4">
       <c r="A3382" t="s">
         <v>6765</v>
       </c>
@@ -49990,7 +50121,7 @@
         <v>6766</v>
       </c>
     </row>
-    <row r="3383" spans="1:2">
+    <row r="3383" spans="1:4">
       <c r="A3383" t="s">
         <v>6767</v>
       </c>
@@ -49998,7 +50129,7 @@
         <v>6768</v>
       </c>
     </row>
-    <row r="3384" spans="1:2">
+    <row r="3384" spans="1:4">
       <c r="A3384" t="s">
         <v>6769</v>
       </c>
@@ -50006,7 +50137,7 @@
         <v>6770</v>
       </c>
     </row>
-    <row r="3385" spans="1:2">
+    <row r="3385" spans="1:4">
       <c r="A3385" t="s">
         <v>6771</v>
       </c>
@@ -50014,7 +50145,7 @@
         <v>6772</v>
       </c>
     </row>
-    <row r="3386" spans="1:2">
+    <row r="3386" spans="1:4">
       <c r="A3386" t="s">
         <v>6773</v>
       </c>
@@ -50022,7 +50153,7 @@
         <v>6774</v>
       </c>
     </row>
-    <row r="3387" spans="1:2">
+    <row r="3387" spans="1:4">
       <c r="A3387" t="s">
         <v>6775</v>
       </c>
@@ -50030,7 +50161,7 @@
         <v>6776</v>
       </c>
     </row>
-    <row r="3388" spans="1:2">
+    <row r="3388" spans="1:4">
       <c r="A3388" t="s">
         <v>6777</v>
       </c>
@@ -50038,7 +50169,7 @@
         <v>6778</v>
       </c>
     </row>
-    <row r="3389" spans="1:2">
+    <row r="3389" spans="1:4">
       <c r="A3389" t="s">
         <v>6779</v>
       </c>
@@ -50046,7 +50177,7 @@
         <v>6780</v>
       </c>
     </row>
-    <row r="3390" spans="1:2">
+    <row r="3390" spans="1:4">
       <c r="A3390" t="s">
         <v>6781</v>
       </c>
@@ -50054,15 +50185,21 @@
         <v>6782</v>
       </c>
     </row>
-    <row r="3391" spans="1:2">
+    <row r="3391" spans="1:4">
       <c r="A3391" t="s">
         <v>6783</v>
       </c>
       <c r="B3391" t="s">
         <v>6784</v>
       </c>
-    </row>
-    <row r="3392" spans="1:2">
+      <c r="C3391" t="s">
+        <v>7501</v>
+      </c>
+      <c r="D3391" t="s">
+        <v>7518</v>
+      </c>
+    </row>
+    <row r="3392" spans="1:4">
       <c r="A3392" t="s">
         <v>6785</v>
       </c>
@@ -52929,6 +53066,7 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>